<commit_message>
[Feature] add extract Excel from LogisticExpenseByProductTemplate #2
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/LogisticExpenseProductTemplate.xlsx
+++ b/src/main/resources/templates/LogisticExpenseProductTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93643669-711E-4BAF-B4A3-347AE38668BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E55E2B-2BEE-418D-8C6E-354A0C31BB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>zoneArea</t>
   </si>
@@ -43,28 +43,7 @@
     <t>status</t>
   </si>
   <si>
-    <t>1263</t>
-  </si>
-  <si>
     <t>BKK1</t>
-  </si>
-  <si>
-    <t>BKK2</t>
-  </si>
-  <si>
-    <t>BKK3</t>
-  </si>
-  <si>
-    <t>BKK4</t>
-  </si>
-  <si>
-    <t>BKK5</t>
-  </si>
-  <si>
-    <t>BKK6</t>
-  </si>
-  <si>
-    <t>BKK7</t>
   </si>
   <si>
     <t>ซี่โครงหมูอ่อนหั่นชิ้นอนามัยซ</t>
@@ -143,12 +122,15 @@
       <t>/** ข้อมูลที่เป็น text ให้ใส่ ' ไว้ข้างหน้าเสมอ เช่น '1263 **/</t>
     </r>
   </si>
+  <si>
+    <t>2910</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +154,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -488,12 +476,13 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -519,171 +508,172 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" s="3">
-        <v>44364</v>
+        <v>45177</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>2.5</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="3">
-        <v>44364</v>
+        <v>45177</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="3">
-        <v>44364</v>
+        <v>45177</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F4">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3">
+        <v>45177</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
-        <v>44364</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
       <c r="F5">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="3">
-        <v>44364</v>
+        <v>45177</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
       <c r="C7" s="3">
-        <v>44364</v>
+        <v>45177</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
       <c r="C8" s="3">
-        <v>44364</v>
+        <v>45177</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>5.5</v>
+      </c>
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="F8">
-        <v>2.5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <customProperties>

</xml_diff>